<commit_message>
Updating documentation and better understanding variables.
</commit_message>
<xml_diff>
--- a/health_data/src/my_dictionary_v2.xlsx
+++ b/health_data/src/my_dictionary_v2.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>variable</t>
   </si>
@@ -42,7 +42,10 @@
     <t>type</t>
   </si>
   <si>
-    <t>notes</t>
+    <t>official_notes</t>
+  </si>
+  <si>
+    <t>researcher_notes</t>
   </si>
   <si>
     <t>premature_death</t>
@@ -57,7 +60,19 @@
     <t xml:space="preserve">National Center for Health Statistics; National Vital Statistics System</t>
   </si>
   <si>
+    <t xml:space="preserve">Cumulative number of years of potential life lost from deaths among county residents under age 75 (summed over three years).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aggregate population under age 75 (over the three years) using bridged--race-postcensal estimates released by NCHS.</t>
+  </si>
+  <si>
     <t>rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data on deaths and births were provided by NCHS and drawn from the NVSS. These data are submitted to the NVSS by the vital registration systems operated in the jurisdictions legally responsible for registering vital events. Usually this variable is calculated by the NCHS, but more recently it has been calculated by the University of Wisconsin Population Health Institute directly using  the Mortality-All County micro-data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Starting in 2020, each observation gets marked as unreliable or suppressed. A value of 0 means no flag is set, a value of 1 means the value is unreliable (based on death counts of 20 or less), and a value of 2 means the value was suppressed (9 or fewer deaths). As far as I can tell, earlier unreliable values are not reported as such.</t>
   </si>
 </sst>
 </file>
@@ -624,14 +639,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" min="1" max="1" style="1" width="15.68359375"/>
+    <col bestFit="1" customWidth="1" min="1" max="1" style="1" width="15.8515625"/>
     <col bestFit="1" customWidth="1" min="2" max="2" style="1" width="33.50390625"/>
     <col bestFit="1" min="3" max="3" style="1" width="7.1015625"/>
     <col customWidth="1" min="4" max="4" style="1" width="17.00390625"/>
-    <col bestFit="1" min="5" max="5" style="1" width="10.140625"/>
-    <col bestFit="1" min="6" max="6" style="1" width="12.140625"/>
+    <col bestFit="1" customWidth="1" min="5" max="5" style="1" width="28.57421875"/>
+    <col bestFit="1" customWidth="1" min="6" max="6" style="1" width="29.57421875"/>
     <col bestFit="1" customWidth="1" min="7" max="7" style="1" width="12.4140625"/>
-    <col min="8" max="16384" style="1" width="9.140625"/>
+    <col bestFit="1" min="8" max="8" style="1" width="8.421875"/>
+    <col bestFit="1" min="9" max="9" style="1" width="4.57421875"/>
+    <col customWidth="1" min="10" max="10" style="1" width="50.00390625"/>
+    <col customWidth="1" min="11" max="11" style="1" width="36.8515625"/>
+    <col min="12" max="16384" style="1" width="9.140625"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="1" ht="14.25">
@@ -665,19 +684,28 @@
       <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" s="1" customFormat="1" ht="57">
-      <c r="A2" s="1" t="s">
-        <v>10</v>
+    <row r="2" s="1" customFormat="1" ht="114">
+      <c r="A2" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="G2" s="1">
         <v>1</v>
@@ -685,8 +713,14 @@
       <c r="H2" s="1">
         <v>0</v>
       </c>
-      <c r="I2" s="3" t="s">
-        <v>14</v>
+      <c r="I2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tired. Read a lot about decomposition of variance. Made some progress on fixing my dictionary.
</commit_message>
<xml_diff>
--- a/health_data/src/my_dictionary_v2.xlsx
+++ b/health_data/src/my_dictionary_v2.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>variable</t>
   </si>
@@ -42,10 +42,13 @@
     <t>type</t>
   </si>
   <si>
-    <t>official_notes</t>
-  </si>
-  <si>
-    <t>researcher_notes</t>
+    <t>note1</t>
+  </si>
+  <si>
+    <t>note2</t>
+  </si>
+  <si>
+    <t>across_time_comparison</t>
   </si>
   <si>
     <t>premature_death</t>
@@ -69,10 +72,64 @@
     <t>rate</t>
   </si>
   <si>
-    <t xml:space="preserve">Data on deaths and births were provided by NCHS and drawn from the NVSS. These data are submitted to the NVSS by the vital registration systems operated in the jurisdictions legally responsible for registering vital events. Usually this variable is calculated by the NCHS, but more recently it has been calculated by the University of Wisconsin Population Health Institute directly using  the Mortality-All County micro-data.</t>
+    <t xml:space="preserve">Data on deaths and births were provided by NCHS and drawn from the NVSS. These data are submitted to the NVSS by the vital registration systems operated in the jurisdictions legally responsible for registering vital events. Usually this variable is calculated by the NCHS, but more recently it has been calculated by the University of Wisconsin Population Health Institute directly using the Mortality-All County micro-data.</t>
   </si>
   <si>
     <t xml:space="preserve">Starting in 2020, each observation gets marked as unreliable or suppressed. A value of 0 means no flag is set, a value of 1 means the value is unreliable (based on death counts of 20 or less), and a value of 2 means the value was suppressed (9 or fewer deaths). As far as I can tell, earlier unreliable values are not reported as such.</t>
+  </si>
+  <si>
+    <t>poor_or_fair_health</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percentage of adults reporting fair or poor health (age-adjusted).</t>
+  </si>
+  <si>
+    <t>brfss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">behavioral risk factor surveillance system</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The numerator is the total number of respondents who answered "Would you say that in general your health is Excellent/Very good/Good/Fair/Poor?" with fair or poor.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The denominator is the total number of adult respondents in a county.</t>
+  </si>
+  <si>
+    <t>percent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRFSS is a state-based random digit dial telephone survey that is conducted annually in all states, the District of Columbia, and U.S. territories. Data obtained from the BRFSS are representative of each state’s total non-institutionalized population over 18 years of age. Data are weighted using iterative proportional fitting (also called "raking") methods to reflect population distributions. Measures are age-adjusted to the 2000 U.S. standard population.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prior to the 2016 County Health Rankings, up to seven survey years of landline only BRFSS data were aggregated to produce county estimates. For the 2016 County Health Rankings and beyond, the CDC produced county estimates using single-year BRFSS data and a multilevel modeling approach based on respondent answers and their age, sex, and race/ethnicity, combined with county-level poverty, as well as county- and state-level contextual effects. To produce estimates for those counties where there were no or limited data, the modeling approach borrowed information from the entire BRFSS sample as well as Census Vintage population estimates. CDC used a parametric bootstrapping method to produce standard errors and confidence intervals for those point estimates. This estimation methodology was validated for all U.S. counties, including those with no or small (&lt; 50 respondents) samples. For the 2021 Rankings, the CDC has updated their modeling procedure for producing small-area estimates. With the PLACES project, a multilevel statistical modeling framework using multilevel regression and poststratification (MRP) is performed for small-area estimation that links BRFSS data with high spatial resolution population demographic and socioeconomic data from the Census’ American Community Survey (ACS). The CDC has performed internal and external validation studies, which confirm strong consistency between their model-based estimates and the direct BRFSS survey estimates at both the state and county levels.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data provider recommends the following time comparisons: 2010-2015; 2016-2020; 2021-2023. Descriptively, the only disjunctures I see are between 2022 and 2023.</t>
+  </si>
+  <si>
+    <t>poor_physical_health_days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poor Physical Health Days measures the average number of physically unhealthy days reported in the past 30 days. This measure is based on responses to the Behavioral Risk Factor Surveillance System (BRFSS) question: “Now thinking about your physical health, which includes physical illness and injury, for how many days during the past 30 days was your physical health not good?”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The total number of days reported by respondents as them experiencing poor physical health.</t>
+  </si>
+  <si>
+    <t>average</t>
+  </si>
+  <si>
+    <t>poor_mental_health_days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poor Mental Health Days measures the average number of mentally unhealthy days reported in past 30 days.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The numerator is the number of days respondents reported to the question "Now thinking about your mental health, which includes stress, depression, and problems with emotions, for how many days during the past 30 days was your mental health not good?"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data provider recommends the following time comparisons: 2010-2015; 2016-2020; 2021-2023. Descriptively, I see no obvious disjunctures in the data.</t>
   </si>
 </sst>
 </file>
@@ -102,7 +159,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -110,20 +167,53 @@
       <bottom style="none"/>
       <diagonal style="none"/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -632,95 +722,216 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A1" zoomScale="100" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" min="1" max="1" style="1" width="15.8515625"/>
+    <col bestFit="1" customWidth="1" min="1" max="1" style="2" width="24.203125"/>
     <col bestFit="1" customWidth="1" min="2" max="2" style="1" width="33.50390625"/>
-    <col bestFit="1" min="3" max="3" style="1" width="7.1015625"/>
+    <col bestFit="1" min="3" max="3" style="1" width="7.3828125"/>
     <col customWidth="1" min="4" max="4" style="1" width="17.00390625"/>
     <col bestFit="1" customWidth="1" min="5" max="5" style="1" width="28.57421875"/>
     <col bestFit="1" customWidth="1" min="6" max="6" style="1" width="29.57421875"/>
-    <col bestFit="1" customWidth="1" min="7" max="7" style="1" width="12.4140625"/>
-    <col bestFit="1" min="8" max="8" style="1" width="8.421875"/>
-    <col bestFit="1" min="9" max="9" style="1" width="4.57421875"/>
+    <col bestFit="1" customWidth="1" min="7" max="7" style="2" width="12.4140625"/>
+    <col bestFit="1" min="8" max="8" style="2" width="8.421875"/>
+    <col bestFit="1" customWidth="1" min="9" max="9" style="2" width="7.54296875"/>
     <col customWidth="1" min="10" max="10" style="1" width="50.00390625"/>
-    <col customWidth="1" min="11" max="11" style="1" width="36.8515625"/>
-    <col min="12" max="16384" style="1" width="9.140625"/>
+    <col bestFit="1" customWidth="1" min="11" max="11" style="1" width="74.203125"/>
+    <col bestFit="1" min="12" max="12" style="1" width="22.30078125"/>
+    <col min="13" max="16384" style="1" width="9.140625"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="1" ht="14.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="3" customFormat="1" ht="14.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" ht="114">
-      <c r="A2" s="3" t="s">
-        <v>11</v>
+      <c r="A2" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="1">
+      <c r="F2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="2">
         <v>1</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="2">
         <v>0</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="J2" s="4" t="s">
         <v>19</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" ht="270.75">
+      <c r="A3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="2">
+        <v>1</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" ht="270.75">
+      <c r="A4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="H4" s="2">
+        <v>1</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" ht="270.75">
+      <c r="A5" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>